<commit_message>
feat(table): premium polish pass and pricing standardization (H-056)
</commit_message>
<xml_diff>
--- a/configs/table-configs/availabilities-complete.xlsx
+++ b/configs/table-configs/availabilities-complete.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53551F0B-85A2-2644-AFAA-8A3D544B7D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="77840" yWindow="-12000" windowWidth="39540" windowHeight="21920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="77860" yWindow="-8720" windowWidth="39540" windowHeight="21920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Column Definitions" sheetId="1" r:id="rId1"/>
@@ -1109,7 +1109,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>